<commit_message>
Add Node server hours
</commit_message>
<xml_diff>
--- a/project-management/time-tracking/Preston-Buterbaugh.xlsx
+++ b/project-management/time-tracking/Preston-Buterbaugh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\time-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388D98D2-CB7C-46F4-9898-E6D6039D4414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4DA8E9-3D21-48DA-8D6F-ADC4190F2EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Date:</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Semester wrap-up meeting, discuss plans for end of semester, schedule for next semester</t>
+  </si>
+  <si>
+    <t>Created Node server, ported Flask server functionality to Node</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -554,7 +557,7 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(B2:B1000)</f>
-        <v>40</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -918,6 +921,17 @@
       </c>
       <c r="C37" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="5">
+        <v>45636</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add repo update hours
</commit_message>
<xml_diff>
--- a/project-management/time-tracking/Preston-Buterbaugh.xlsx
+++ b/project-management/time-tracking/Preston-Buterbaugh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\time-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4DA8E9-3D21-48DA-8D6F-ADC4190F2EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126706B8-47FC-435B-B950-C1E59C4660A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Date:</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Created Node server, ported Flask server functionality to Node</t>
+  </si>
+  <si>
+    <t>Merge pull request, general repository organization</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -557,7 +560,7 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(B2:B1000)</f>
-        <v>41.5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -932,6 +935,17 @@
       </c>
       <c r="C38" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="5">
+        <v>45638</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add resource review hours
</commit_message>
<xml_diff>
--- a/project-management/time-tracking/Preston-Buterbaugh.xlsx
+++ b/project-management/time-tracking/Preston-Buterbaugh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\time-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126706B8-47FC-435B-B950-C1E59C4660A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5445627D-2ADB-44E7-AC41-762411D5C926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Date:</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Merge pull request, general repository organization</t>
+  </si>
+  <si>
+    <t>Review callstack and architecture resources</t>
+  </si>
+  <si>
+    <t>Review assembly code resources</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -560,7 +566,7 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(B2:B1000)</f>
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -946,6 +952,28 @@
       </c>
       <c r="C39" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="5">
+        <v>45639</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="5">
+        <v>45639</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add time tracking and hour summaries
</commit_message>
<xml_diff>
--- a/project-management/time-tracking/Preston-Buterbaugh.xlsx
+++ b/project-management/time-tracking/Preston-Buterbaugh.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\time-tracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 8 (Spring 2025)\CS 5002 - Senior Design II\senior-design\project-management\time-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5445627D-2ADB-44E7-AC41-762411D5C926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1780607A-8CFB-4CCD-BE57-7E506BC0DA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Preston" sheetId="1" r:id="rId1"/>
+    <sheet name="Fall 2024" sheetId="1" r:id="rId1"/>
+    <sheet name="Spring 2025" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
   <si>
     <t>Date:</t>
   </si>
@@ -162,6 +163,162 @@
   </si>
   <si>
     <t>Review assembly code resources</t>
+  </si>
+  <si>
+    <t>Complete team registration form for CEAS Expo</t>
+  </si>
+  <si>
+    <t>Set up Virtual Machine as runtime environment for Hackademia</t>
+  </si>
+  <si>
+    <t>Discuss methods of disassembling machine code with advisor</t>
+  </si>
+  <si>
+    <t>Experiment with compiling C code and inspecting output patterns</t>
+  </si>
+  <si>
+    <t>Investigated new server implementation</t>
+  </si>
+  <si>
+    <t>C code compilation process</t>
+  </si>
+  <si>
+    <t>Discuss frontend style library options with advisor</t>
+  </si>
+  <si>
+    <t>Team meeting to discuss progress and hold-ups, work on C code compilation process</t>
+  </si>
+  <si>
+    <t>Met with Pratik to discuss new server implementation</t>
+  </si>
+  <si>
+    <t>Team meeting to discuss new server structure, class assignments, and plans for further development</t>
+  </si>
+  <si>
+    <t>Implement "compile" API route</t>
+  </si>
+  <si>
+    <t>Review test plan</t>
+  </si>
+  <si>
+    <t>Implement C code compilation process</t>
+  </si>
+  <si>
+    <t>Integrated C code compilation with client changes and discussed future development plans</t>
+  </si>
+  <si>
+    <t>User Documentation</t>
+  </si>
+  <si>
+    <t>Time Tracking</t>
+  </si>
+  <si>
+    <t>Update compilation function to handle multiple functions of C code</t>
+  </si>
+  <si>
+    <t>Meet to sync up with team and discuss upcoming work assignments and homework tasks</t>
+  </si>
+  <si>
+    <t>Refactor code for Dynamic Callstack Component</t>
+  </si>
+  <si>
+    <t>Work on Expo slide deck</t>
+  </si>
+  <si>
+    <t>Reviewed progress and plans to interpret assembly code with advisor</t>
+  </si>
+  <si>
+    <t>Added 32-bit compilation and better error handling</t>
+  </si>
+  <si>
+    <t>Fix issues with library includes and filtering for functions when compiling 32-bit code</t>
+  </si>
+  <si>
+    <t>Meeting to sync up with the rest of the team and discuss how to merge divergent branches of work</t>
+  </si>
+  <si>
+    <t>Troubleshot and fixed filtering of 32-bit functions</t>
+  </si>
+  <si>
+    <t>Add basic information to expo poster</t>
+  </si>
+  <si>
+    <t>Researched assembly instructions and discussed project progress with team</t>
+  </si>
+  <si>
+    <t>Discuss methods of emulating assembly instructions and displaying memory values with advisor</t>
+  </si>
+  <si>
+    <t>Researched assembly instructions</t>
+  </si>
+  <si>
+    <t>Team meeting to sync up on tasks and troubleshoot environments</t>
+  </si>
+  <si>
+    <t>Work on parsing assembly instructions to determine proper implementation</t>
+  </si>
+  <si>
+    <t>Reviewed expo poster design</t>
+  </si>
+  <si>
+    <t>Experiment with assembly instruction implementation</t>
+  </si>
+  <si>
+    <t>Team meeting to sync up on tasks and determine work to be completed before expo</t>
+  </si>
+  <si>
+    <t>Investigated available information for each assembly instruction from the Iced API</t>
+  </si>
+  <si>
+    <t>Met with advisor to discuss best ways of getting operands of each assembly instruction</t>
+  </si>
+  <si>
+    <t>Implement case structure to parse and emulate common assembly instructions</t>
+  </si>
+  <si>
+    <t>Meet to sync up with team on tasks and plan work to be done over spring break</t>
+  </si>
+  <si>
+    <t>Implemented structures to handle different data type numbers, and unsupported instructions</t>
+  </si>
+  <si>
+    <t>Implement POP and ADD instructions</t>
+  </si>
+  <si>
+    <t>Investigate Iced handling of memory addresses, and set up instruction pointer</t>
+  </si>
+  <si>
+    <t>Refine disassembly process to associate address and state with each instruction</t>
+  </si>
+  <si>
+    <t>Met to sync up with team on tasks that had been accomplished over spring break, and work to be done</t>
+  </si>
+  <si>
+    <t>Resolve merge conflict</t>
+  </si>
+  <si>
+    <t>Implement 32-bit register operations for 64-bit assembly code</t>
+  </si>
+  <si>
+    <t>Troubleshoot state updating after each instruction</t>
+  </si>
+  <si>
+    <t>Met with advisor to discuss project status and plans before expo</t>
+  </si>
+  <si>
+    <t>Unified work from various team members tasks, discussed final action items before the expo</t>
+  </si>
+  <si>
+    <t>Divided final report work and continued work on associating addresses with each instruction</t>
+  </si>
+  <si>
+    <t>Discussed final report work and troubleshot final errors</t>
+  </si>
+  <si>
+    <t>Implemented proper stack visualization for values that are stored relative to the base pointer</t>
+  </si>
+  <si>
+    <t>Final self assessment and report updates</t>
   </si>
 </sst>
 </file>
@@ -504,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -979,4 +1136,672 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F9426B-3C22-47EF-863F-ED33066D4816}">
+  <dimension ref="A1:F58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="13.3125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.83984375" style="1"/>
+    <col min="3" max="3" width="85.9453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83984375" style="1"/>
+    <col min="5" max="5" width="15.3125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="5">
+        <v>45670</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5">
+        <v>45672</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5">
+        <v>45672</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <f>SUM(B2:B1000)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5">
+        <v>45673</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5">
+        <v>45674</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5">
+        <v>45674</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5">
+        <v>45675</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5">
+        <v>45676</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5">
+        <v>45679</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5">
+        <v>45680</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5">
+        <v>45680</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5">
+        <v>45681</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="5">
+        <v>45687</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="5">
+        <v>45687</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="5">
+        <v>45690</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="5">
+        <v>45693</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4.25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="5">
+        <v>45694</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="5">
+        <v>45697</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="5">
+        <v>45697</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="5">
+        <v>45700</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="5">
+        <v>45701</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="5">
+        <v>45701</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="5">
+        <v>45702</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="5">
+        <v>45705</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="5">
+        <v>45706</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="5">
+        <v>45707</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="5">
+        <v>45708</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="5">
+        <v>45708</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="5">
+        <v>45712</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="5">
+        <v>45712</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="5">
+        <v>45712</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="5">
+        <v>45714</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="5">
+        <v>45715</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="5">
+        <v>45715</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="5">
+        <v>45718</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="5">
+        <v>45721</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="5">
+        <v>45722</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="5">
+        <v>45725</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3.75</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="5">
+        <v>45726</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="5">
+        <v>45728</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2.75</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="5">
+        <v>45729</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="5">
+        <v>45734</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="5">
+        <v>45734</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="5">
+        <v>45735</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="5">
+        <v>45736</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="5">
+        <v>45742</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="5">
+        <v>45746</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="5">
+        <v>45747</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2.25</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="5">
+        <v>45747</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="5">
+        <v>45747</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="5">
+        <v>45748</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="5">
+        <v>45750</v>
+      </c>
+      <c r="B53" s="1">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="5">
+        <v>45750</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="5">
+        <v>45753</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="5">
+        <v>45754</v>
+      </c>
+      <c r="B56" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="5">
+        <v>45754</v>
+      </c>
+      <c r="B57" s="1">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="5">
+        <v>45761</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>